<commit_message>
updated core ABM model
</commit_message>
<xml_diff>
--- a/fears_md/data/pharmacodynamics_library.xlsx
+++ b/fears_md/data/pharmacodynamics_library.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinge2/repos/fears_md/fears_md/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eshanking/repos/fears_md/fears_md/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DC7D82-56D4-DB42-9363-25132545100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47CE4B4-AB3C-D44D-9A8F-BDC53858C308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="7980" windowWidth="28040" windowHeight="17440" xr2:uid="{F8A24BF3-E3AE-3649-AED6-C649CF1E17FC}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15960" xr2:uid="{F8A24BF3-E3AE-3649-AED6-C649CF1E17FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -114,9 +115,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -154,7 +155,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -260,7 +261,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -402,7 +403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360E22EC-FC85-C04A-8F00-5C0990B63ABF}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,17 +444,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D2">
-        <f ca="1">10^(RAND()*3)</f>
-        <v>15.011841515973286</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -464,17 +464,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" ca="1" si="0">10^(RAND()*3)</f>
-        <v>102.48764701912289</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -485,17 +484,16 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>27.612562855139764</v>
+        <v>100</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -506,17 +504,16 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>18.196348338649887</v>
+        <v>1000</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -527,17 +524,16 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>16.231627504120873</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -548,17 +544,16 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>15.631642982280962</v>
+        <v>100</v>
       </c>
       <c r="E7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -569,17 +564,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.2187537615590527</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -590,17 +584,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="0"/>
-        <v>207.02327683027713</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>3</v>

</xml_diff>